<commit_message>
003: Added several apps
</commit_message>
<xml_diff>
--- a/backend/indexes/management/commands/t_indexes_actual.xlsx
+++ b/backend/indexes/management/commands/t_indexes_actual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahir\OneDrive\Desktop\Codes\YKHT\backend\indexes\management\commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{551B0326-CE9E-4C73-BF82-ED158799ABDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4704AC6-C7FA-4744-81F1-04052B695893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\ \-\ mm\ \-\ dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\ \-\ mm\ \-\ dd"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -93,12 +93,14 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
       <charset val="162"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
       <charset val="162"/>
     </font>
     <font>
@@ -204,7 +206,7 @@
     <xf numFmtId="4" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -518,7 +520,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,35 +623,35 @@
       <c r="A3" s="2">
         <v>44562</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
+      <c r="B3">
+        <v>763.23</v>
+      </c>
+      <c r="C3">
+        <v>412.31</v>
+      </c>
+      <c r="D3">
+        <v>2495.39</v>
+      </c>
+      <c r="E3">
+        <v>3041.94</v>
+      </c>
+      <c r="F3">
+        <v>2691.46</v>
+      </c>
+      <c r="G3">
+        <v>877.87</v>
+      </c>
+      <c r="H3">
+        <v>953.84</v>
+      </c>
+      <c r="I3">
+        <v>792.77</v>
+      </c>
+      <c r="J3">
+        <v>1129.03</v>
+      </c>
+      <c r="K3">
+        <v>816.45</v>
       </c>
       <c r="L3" s="1">
         <v>15.322900000000001</v>
@@ -659,42 +661,42 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N32" si="0">+_xlfn.TEXTJOIN(";",2,A3:M3)</f>
-        <v>44562;0;0;0;0;0;0;0;0;0;0;15.3229;13.5348</v>
+        <v>44562;763.23;412.31;2495.39;3041.94;2691.46;877.87;953.84;792.77;1129.03;816.45;15.3229;13.5348</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44593</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
+      <c r="B4">
+        <v>799.93</v>
+      </c>
+      <c r="C4">
+        <v>453.56</v>
+      </c>
+      <c r="D4">
+        <v>2568.25</v>
+      </c>
+      <c r="E4">
+        <v>3228.45</v>
+      </c>
+      <c r="F4">
+        <v>3024.19</v>
+      </c>
+      <c r="G4">
+        <v>960.44</v>
+      </c>
+      <c r="H4">
+        <v>994.81</v>
+      </c>
+      <c r="I4">
+        <v>784.2</v>
+      </c>
+      <c r="J4">
+        <v>1210.5999999999999</v>
+      </c>
+      <c r="K4">
+        <v>845.24</v>
       </c>
       <c r="L4" s="1">
         <v>15.483000000000001</v>
@@ -704,42 +706,42 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
-        <v>44593;0;0;0;0;0;0;0;0;0;0;15.483;13.6547</v>
+        <v>44593;799.93;453.56;2568.25;3228.45;3024.19;960.44;994.81;784.2;1210.6;845.24;15.483;13.6547</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44621</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
+      <c r="B5">
+        <v>843.64</v>
+      </c>
+      <c r="C5">
+        <v>502.06</v>
+      </c>
+      <c r="D5">
+        <v>2878.66</v>
+      </c>
+      <c r="E5">
+        <v>3592.1</v>
+      </c>
+      <c r="F5">
+        <v>4118.83</v>
+      </c>
+      <c r="G5">
+        <v>1018.77</v>
+      </c>
+      <c r="H5">
+        <v>1054.23</v>
+      </c>
+      <c r="I5">
+        <v>789.65</v>
+      </c>
+      <c r="J5">
+        <v>1321.9</v>
+      </c>
+      <c r="K5">
+        <v>879.21</v>
       </c>
       <c r="L5" s="1">
         <v>16.1005</v>
@@ -749,42 +751,42 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
-        <v>44621;0;0;0;0;0;0;0;0;0;0;16.1005;14.6139</v>
+        <v>44621;843.64;502.06;2878.66;3592.1;4118.83;1018.77;1054.23;789.65;1321.9;879.21;16.1005;14.6139</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44652</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
+      <c r="B6">
+        <v>904.79</v>
+      </c>
+      <c r="C6">
+        <v>542.12</v>
+      </c>
+      <c r="D6">
+        <v>3069.68</v>
+      </c>
+      <c r="E6">
+        <v>3785.55</v>
+      </c>
+      <c r="F6">
+        <v>4257.26</v>
+      </c>
+      <c r="G6">
+        <v>1110.9100000000001</v>
+      </c>
+      <c r="H6">
+        <v>1086.8699999999999</v>
+      </c>
+      <c r="I6">
+        <v>807.96</v>
+      </c>
+      <c r="J6">
+        <v>1423.27</v>
+      </c>
+      <c r="K6">
+        <v>902.82</v>
       </c>
       <c r="L6" s="1">
         <v>15.9145</v>
@@ -794,42 +796,42 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>44652;0;0;0;0;0;0;0;0;0;0;15.9145;14.7037</v>
+        <v>44652;904.79;542.12;3069.68;3785.55;4257.26;1110.91;1086.87;807.96;1423.27;902.82;15.9145;14.7037</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44682</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
+      <c r="B7">
+        <v>931.76</v>
+      </c>
+      <c r="C7">
+        <v>564.41999999999996</v>
+      </c>
+      <c r="D7">
+        <v>3183.54</v>
+      </c>
+      <c r="E7">
+        <v>3734.86</v>
+      </c>
+      <c r="F7">
+        <v>4551.93</v>
+      </c>
+      <c r="G7">
+        <v>1194.3900000000001</v>
+      </c>
+      <c r="H7">
+        <v>1124.7</v>
+      </c>
+      <c r="I7">
+        <v>856.25</v>
+      </c>
+      <c r="J7">
+        <v>1548.01</v>
+      </c>
+      <c r="K7">
+        <v>945.82</v>
       </c>
       <c r="L7" s="1">
         <v>16.6343</v>
@@ -839,42 +841,42 @@
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
-        <v>44682;0;0;0;0;0;0;0;0;0;0;16.6343;15.7197</v>
+        <v>44682;931.76;564.42;3183.54;3734.86;4551.93;1194.39;1124.7;856.25;1548.01;945.82;16.6343;15.7197</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44713</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
+      <c r="B8">
+        <v>977.9</v>
+      </c>
+      <c r="C8">
+        <v>595.41999999999996</v>
+      </c>
+      <c r="D8">
+        <v>3279.12</v>
+      </c>
+      <c r="E8">
+        <v>3915.44</v>
+      </c>
+      <c r="F8">
+        <v>5691.23</v>
+      </c>
+      <c r="G8">
+        <v>1274.9100000000001</v>
+      </c>
+      <c r="H8">
+        <v>1192.25</v>
+      </c>
+      <c r="I8">
+        <v>936.45</v>
+      </c>
+      <c r="J8">
+        <v>1652.75</v>
+      </c>
+      <c r="K8">
+        <v>1006.95</v>
       </c>
       <c r="L8" s="1">
         <v>17.9681</v>
@@ -884,42 +886,42 @@
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v>44713;0;0;0;0;0;0;0;0;0;0;17.9681;16.9924</v>
+        <v>44713;977.9;595.42;3279.12;3915.44;5691.23;1274.91;1192.25;936.45;1652.75;1006.95;17.9681;16.9924</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44743</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
+      <c r="B9">
+        <v>1001.03</v>
+      </c>
+      <c r="C9">
+        <v>610.26</v>
+      </c>
+      <c r="D9">
+        <v>3190.01</v>
+      </c>
+      <c r="E9">
+        <v>3653.13</v>
+      </c>
+      <c r="F9">
+        <v>5177.63</v>
+      </c>
+      <c r="G9">
+        <v>1318.77</v>
+      </c>
+      <c r="H9">
+        <v>1232.6300000000001</v>
+      </c>
+      <c r="I9">
+        <v>969.92</v>
+      </c>
+      <c r="J9">
+        <v>1738.21</v>
+      </c>
+      <c r="K9">
+        <v>1045.22</v>
       </c>
       <c r="L9" s="1">
         <v>17.8537</v>
@@ -929,42 +931,42 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
-        <v>44743;0;0;0;0;0;0;0;0;0;0;17.8537;17.4831</v>
+        <v>44743;1001.03;610.26;3190.01;3653.13;5177.63;1318.77;1232.63;969.92;1738.21;1045.22;17.8537;17.4831</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44774</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
+      <c r="B10">
+        <v>1015.65</v>
+      </c>
+      <c r="C10">
+        <v>624.30999999999995</v>
+      </c>
+      <c r="D10">
+        <v>3108.9</v>
+      </c>
+      <c r="E10">
+        <v>3856.15</v>
+      </c>
+      <c r="F10">
+        <v>4875.6499999999996</v>
+      </c>
+      <c r="G10">
+        <v>1373.36</v>
+      </c>
+      <c r="H10">
+        <v>1262.8699999999999</v>
+      </c>
+      <c r="I10">
+        <v>985.05</v>
+      </c>
+      <c r="J10">
+        <v>1780.05</v>
+      </c>
+      <c r="K10">
+        <v>1080.3</v>
       </c>
       <c r="L10" s="1">
         <v>18.2622</v>
@@ -974,42 +976,42 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
-        <v>44774;0;0;0;0;0;0;0;0;0;0;18.2622;18.0237</v>
+        <v>44774;1015.65;624.31;3108.9;3856.15;4875.65;1373.36;1262.87;985.05;1780.05;1080.3;18.2622;18.0237</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44805</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
+      <c r="B11">
+        <v>1046.8900000000001</v>
+      </c>
+      <c r="C11">
+        <v>659.25</v>
+      </c>
+      <c r="D11">
+        <v>3132.95</v>
+      </c>
+      <c r="E11">
+        <v>3794.03</v>
+      </c>
+      <c r="F11">
+        <v>4736.3100000000004</v>
+      </c>
+      <c r="G11">
+        <v>1400.14</v>
+      </c>
+      <c r="H11">
+        <v>1297.8399999999999</v>
+      </c>
+      <c r="I11">
+        <v>1000.81</v>
+      </c>
+      <c r="J11">
+        <v>1865.09</v>
+      </c>
+      <c r="K11">
+        <v>1103.6099999999999</v>
       </c>
       <c r="L11" s="1">
         <v>18.144200000000001</v>
@@ -1019,42 +1021,42 @@
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
-        <v>44805;0;0;0;0;0;0;0;0;0;0;18.1442;18.3137</v>
+        <v>44805;1046.89;659.25;3132.95;3794.03;4736.31;1400.14;1297.84;1000.81;1865.09;1103.61;18.1442;18.3137</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44835</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
+      <c r="B12">
+        <v>1084</v>
+      </c>
+      <c r="C12">
+        <v>686.76</v>
+      </c>
+      <c r="D12">
+        <v>3143.79</v>
+      </c>
+      <c r="E12">
+        <v>3820.51</v>
+      </c>
+      <c r="F12">
+        <v>5034.41</v>
+      </c>
+      <c r="G12">
+        <v>1430.51</v>
+      </c>
+      <c r="H12">
+        <v>1318.66</v>
+      </c>
+      <c r="I12">
+        <v>1024.52</v>
+      </c>
+      <c r="J12">
+        <v>2011.13</v>
+      </c>
+      <c r="K12">
+        <v>1148.3</v>
       </c>
       <c r="L12" s="1">
         <v>18.261199999999999</v>
@@ -1064,42 +1066,42 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
-        <v>44835;0;0;0;0;0;0;0;0;0;0;18.2612;18.5838</v>
+        <v>44835;1084;686.76;3143.79;3820.51;5034.41;1430.51;1318.66;1024.52;2011.13;1148.3;18.2612;18.5838</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44866</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
+      <c r="B13">
+        <v>1115.26</v>
+      </c>
+      <c r="C13">
+        <v>707.69</v>
+      </c>
+      <c r="D13">
+        <v>3121.86</v>
+      </c>
+      <c r="E13">
+        <v>3920.18</v>
+      </c>
+      <c r="F13">
+        <v>4932.09</v>
+      </c>
+      <c r="G13">
+        <v>1430.62</v>
+      </c>
+      <c r="H13">
+        <v>1366.38</v>
+      </c>
+      <c r="I13">
+        <v>1046.04</v>
+      </c>
+      <c r="J13">
+        <v>2026.08</v>
+      </c>
+      <c r="K13">
+        <v>1180.23</v>
       </c>
       <c r="L13" s="1">
         <v>18.9742</v>
@@ -1109,42 +1111,42 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
-        <v>44866;0;0;0;0;0;0;0;0;0;0;18.9742;18.6089</v>
+        <v>44866;1115.26;707.69;3121.86;3920.18;4932.09;1430.62;1366.38;1046.04;2026.08;1180.23;18.9742;18.6089</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44896</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
+      <c r="B14">
+        <v>1128.45</v>
+      </c>
+      <c r="C14">
+        <v>715.3</v>
+      </c>
+      <c r="D14">
+        <v>3151.41</v>
+      </c>
+      <c r="E14">
+        <v>4004.73</v>
+      </c>
+      <c r="F14">
+        <v>4312.3599999999997</v>
+      </c>
+      <c r="G14">
+        <v>1430.96</v>
+      </c>
+      <c r="H14">
+        <v>1395.91</v>
+      </c>
+      <c r="I14">
+        <v>1064.8699999999999</v>
+      </c>
+      <c r="J14">
+        <v>2021.19</v>
+      </c>
+      <c r="K14">
+        <v>1204.94</v>
       </c>
       <c r="L14" s="1">
         <v>19.752099999999999</v>
@@ -1154,42 +1156,42 @@
       </c>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
-        <v>44896;0;0;0;0;0;0;0;0;0;0;19.7521;18.6573</v>
+        <v>44896;1128.45;715.3;3151.41;4004.73;4312.36;1430.96;1395.91;1064.87;2021.19;1204.94;19.7521;18.6573</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44927</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
+      <c r="B15">
+        <v>1203.48</v>
+      </c>
+      <c r="C15">
+        <v>754.6</v>
+      </c>
+      <c r="D15">
+        <v>3218.34</v>
+      </c>
+      <c r="E15">
+        <v>4168.4799999999996</v>
+      </c>
+      <c r="F15">
+        <v>4470.3900000000003</v>
+      </c>
+      <c r="G15">
+        <v>1438.91</v>
+      </c>
+      <c r="H15">
+        <v>1440.25</v>
+      </c>
+      <c r="I15">
+        <v>1082.01</v>
+      </c>
+      <c r="J15">
+        <v>2105.17</v>
+      </c>
+      <c r="K15">
+        <v>1305.3900000000001</v>
       </c>
       <c r="L15" s="1">
         <v>20.232600000000001</v>
@@ -1199,42 +1201,42 @@
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
-        <v>44927;0;0;0;0;0;0;0;0;0;0;20.2326;18.7785</v>
+        <v>44927;1203.48;754.6;3218.34;4168.48;4470.39;1438.91;1440.25;1082.01;2105.17;1305.39;20.2326;18.7785</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44958</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
+      <c r="B16">
+        <v>1241.33</v>
+      </c>
+      <c r="C16">
+        <v>778.31</v>
+      </c>
+      <c r="D16">
+        <v>3323.44</v>
+      </c>
+      <c r="E16">
+        <v>4207.6099999999997</v>
+      </c>
+      <c r="F16">
+        <v>4404.82</v>
+      </c>
+      <c r="G16">
+        <v>1471.93</v>
+      </c>
+      <c r="H16">
+        <v>1456.31</v>
+      </c>
+      <c r="I16">
+        <v>1160.31</v>
+      </c>
+      <c r="J16">
+        <v>2138.04</v>
+      </c>
+      <c r="K16">
+        <v>1333.49</v>
       </c>
       <c r="L16" s="1">
         <v>20.195</v>
@@ -1244,42 +1246,42 @@
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
-        <v>44958;0;0;0;0;0;0;0;0;0;0;20.195;18.8441</v>
+        <v>44958;1241.33;778.31;3323.44;4207.61;4404.82;1471.93;1456.31;1160.31;2138.04;1333.49;20.195;18.8441</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44986</v>
       </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
+      <c r="B17">
+        <v>1269.75</v>
+      </c>
+      <c r="C17">
+        <v>791.19</v>
+      </c>
+      <c r="D17">
+        <v>3426.85</v>
+      </c>
+      <c r="E17">
+        <v>4145.7</v>
+      </c>
+      <c r="F17">
+        <v>4194.8</v>
+      </c>
+      <c r="G17">
+        <v>1527.59</v>
+      </c>
+      <c r="H17">
+        <v>1473.18</v>
+      </c>
+      <c r="I17">
+        <v>1185.0999999999999</v>
+      </c>
+      <c r="J17">
+        <v>2147.44</v>
+      </c>
+      <c r="K17">
+        <v>1357.76</v>
       </c>
       <c r="L17" s="1">
         <v>20.343699999999998</v>
@@ -1289,42 +1291,42 @@
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
-        <v>44986;0;0;0;0;0;0;0;0;0;0;20.3437;18.9989</v>
+        <v>44986;1269.75;791.19;3426.85;4145.7;4194.8;1527.59;1473.18;1185.1;2147.44;1357.76;20.3437;18.9989</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45017</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0</v>
+      <c r="B18">
+        <v>1300.04</v>
+      </c>
+      <c r="C18">
+        <v>810.72</v>
+      </c>
+      <c r="D18">
+        <v>3506.86</v>
+      </c>
+      <c r="E18">
+        <v>4225.2700000000004</v>
+      </c>
+      <c r="F18">
+        <v>4206.68</v>
+      </c>
+      <c r="G18">
+        <v>1558.4</v>
+      </c>
+      <c r="H18">
+        <v>1542.72</v>
+      </c>
+      <c r="I18">
+        <v>1200.3399999999999</v>
+      </c>
+      <c r="J18">
+        <v>2164.94</v>
+      </c>
+      <c r="K18">
+        <v>1395.43</v>
       </c>
       <c r="L18" s="1">
         <v>21.1951</v>
@@ -1334,42 +1336,42 @@
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
-        <v>45017;0;0;0;0;0;0;0;0;0;0;21.1951;19.334</v>
+        <v>45017;1300.04;810.72;3506.86;4225.27;4206.68;1558.4;1542.72;1200.34;2164.94;1395.43;21.1951;19.334</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45047</v>
       </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1">
-        <v>0</v>
+      <c r="B19">
+        <v>1300.5999999999999</v>
+      </c>
+      <c r="C19">
+        <v>811.49</v>
+      </c>
+      <c r="D19">
+        <v>3515.08</v>
+      </c>
+      <c r="E19">
+        <v>4200.3100000000004</v>
+      </c>
+      <c r="F19">
+        <v>3843.45</v>
+      </c>
+      <c r="G19">
+        <v>1616.41</v>
+      </c>
+      <c r="H19">
+        <v>1586.5</v>
+      </c>
+      <c r="I19">
+        <v>1209.67</v>
+      </c>
+      <c r="J19">
+        <v>2179.02</v>
+      </c>
+      <c r="K19">
+        <v>1424.63</v>
       </c>
       <c r="L19" s="1">
         <v>21.478000000000002</v>
@@ -1379,42 +1381,42 @@
       </c>
       <c r="N19" t="str">
         <f t="shared" si="0"/>
-        <v>45047;0;0;0;0;0;0;0;0;0;0;21.478;19.7607</v>
+        <v>45047;1300.6;811.49;3515.08;4200.31;3843.45;1616.41;1586.5;1209.67;2179.02;1424.63;21.478;19.7607</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45078</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0</v>
+      <c r="B20">
+        <v>1351.59</v>
+      </c>
+      <c r="C20">
+        <v>826.34</v>
+      </c>
+      <c r="D20">
+        <v>3823.46</v>
+      </c>
+      <c r="E20">
+        <v>4665.91</v>
+      </c>
+      <c r="F20">
+        <v>4541.8100000000004</v>
+      </c>
+      <c r="G20">
+        <v>1696.66</v>
+      </c>
+      <c r="H20">
+        <v>1724.78</v>
+      </c>
+      <c r="I20">
+        <v>1227.55</v>
+      </c>
+      <c r="J20">
+        <v>2320.7199999999998</v>
+      </c>
+      <c r="K20">
+        <v>1526.03</v>
       </c>
       <c r="L20" s="1">
         <v>25.127199999999998</v>
@@ -1424,42 +1426,42 @@
       </c>
       <c r="N20" t="str">
         <f t="shared" si="0"/>
-        <v>45078;0;0;0;0;0;0;0;0;0;0;25.1272;23.2187</v>
+        <v>45078;1351.59;826.34;3823.46;4665.91;4541.81;1696.66;1724.78;1227.55;2320.72;1526.03;25.1272;23.2187</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45108</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
+      <c r="B21">
+        <v>1479.84</v>
+      </c>
+      <c r="C21">
+        <v>897.51</v>
+      </c>
+      <c r="D21">
+        <v>4173.12</v>
+      </c>
+      <c r="E21">
+        <v>5361.27</v>
+      </c>
+      <c r="F21">
+        <v>5462.3</v>
+      </c>
+      <c r="G21">
+        <v>1767.03</v>
+      </c>
+      <c r="H21">
+        <v>2016.7</v>
+      </c>
+      <c r="I21">
+        <v>1309.51</v>
+      </c>
+      <c r="J21">
+        <v>2511.75</v>
+      </c>
+      <c r="K21">
+        <v>1693.95</v>
       </c>
       <c r="L21" s="1">
         <v>29.303999999999998</v>
@@ -1469,41 +1471,41 @@
       </c>
       <c r="N21" t="str">
         <f t="shared" si="0"/>
-        <v>45108;0;0;0;0;0;0;0;0;0;0;29.304;26.4994</v>
+        <v>45108;1479.84;897.51;4173.12;5361.27;5462.3;1767.03;2016.7;1309.51;2511.75;1693.95;29.304;26.4994</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45139</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>1614.31</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>963.83</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>4231.07</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <v>5459.49</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
         <v>6499.71</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22">
         <v>1864.37</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22">
         <v>2084.4</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22">
         <v>1341.07</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22">
         <v>2659.6</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22">
         <v>1762.8</v>
       </c>
       <c r="L22" s="1">
@@ -1521,35 +1523,35 @@
       <c r="A23" s="2">
         <v>45170</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0</v>
+      <c r="B23">
+        <v>1691.04</v>
+      </c>
+      <c r="C23">
+        <v>1008.27</v>
+      </c>
+      <c r="D23">
+        <v>4226.72</v>
+      </c>
+      <c r="E23">
+        <v>5480.31</v>
+      </c>
+      <c r="F23">
+        <v>6891.46</v>
+      </c>
+      <c r="G23">
+        <v>1960.01</v>
+      </c>
+      <c r="H23">
+        <v>2076.7800000000002</v>
+      </c>
+      <c r="I23">
+        <v>1346.22</v>
+      </c>
+      <c r="J23">
+        <v>2749.98</v>
+      </c>
+      <c r="K23">
+        <v>1825.57</v>
       </c>
       <c r="L23" s="1">
         <v>28.847000000000001</v>
@@ -1559,41 +1561,41 @@
       </c>
       <c r="N23" t="str">
         <f t="shared" si="0"/>
-        <v>45170;0;0;0;0;0;0;0;0;0;0;28.847;27.7964</v>
+        <v>45170;1691.04;1008.27;4226.72;5480.31;6891.46;1960.01;2076.78;1346.22;2749.98;1825.57;28.847;27.7964</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45200</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>1749.11</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>1048.26</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>4287.22</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>5517.85</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>6673.74</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24">
         <v>2041.36</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <v>2144.1</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24">
         <v>1378.01</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24">
         <v>2803.29</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24">
         <v>1869.2</v>
       </c>
       <c r="L24" s="1">
@@ -1611,34 +1613,34 @@
       <c r="A25" s="2">
         <v>45231</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>1806.5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>1067.22</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>4376.3599999999997</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <v>5718.08</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>6436.03</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25">
         <v>2129.65</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25">
         <v>2205.67</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25">
         <v>1458.95</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25">
         <v>2882.04</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25">
         <v>1925.23</v>
       </c>
       <c r="L25" s="1">
@@ -1656,34 +1658,34 @@
       <c r="A26" s="2">
         <v>45261</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>1859.38</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>1082.5</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>4517.42</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <v>5849.19</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>6202.52</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <v>2208.3200000000002</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <v>2250.87</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26">
         <v>1487.92</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26">
         <v>2915.02</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26">
         <v>1968.58</v>
       </c>
       <c r="L26" s="1">

</xml_diff>